<commit_message>
GoodInfo_v2 - 2021.12.01 完成
</commit_message>
<xml_diff>
--- a/GoodInfo_StockList_20211201.xlsx
+++ b/GoodInfo_StockList_20211201.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20380"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aaeon365-my.sharepoint.com/personal/raywu_aaeon_com_tw/Documents/_OLD/Documents/Python/GoodInfo_v2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ray\Documents\Python\GoodInfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{68902B30-2F1B-4771-92F4-7FB04DA12068}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -241,7 +240,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -606,11 +605,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -649,53 +648,59 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>1570</v>
+        <v>1721</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D2">
-        <v>25.95</v>
+        <v>30.45</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
       </c>
       <c r="K2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B3">
-        <v>1611</v>
+        <v>3306</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="D3">
-        <v>16.55</v>
+        <v>35.9</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
       </c>
       <c r="K3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="B4">
-        <v>1709</v>
+        <v>6205</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="D4">
-        <v>25.45</v>
+        <v>57.8</v>
       </c>
       <c r="E4">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="K4" t="s">
         <v>11</v>
@@ -703,45 +708,45 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="B5">
-        <v>1712</v>
+        <v>5607</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="D5">
-        <v>28.95</v>
+        <v>60</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
-      <c r="F5">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="H5">
-        <v>1.3</v>
-      </c>
       <c r="K5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>1721</v>
+        <v>1712</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6">
-        <v>30.45</v>
+        <v>28.95</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="H6">
+        <v>1.3</v>
       </c>
       <c r="K6" t="s">
         <v>11</v>
@@ -749,19 +754,25 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>1722</v>
+        <v>2374</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D7">
-        <v>73.2</v>
+        <v>25.45</v>
       </c>
       <c r="E7">
-        <v>2.8</v>
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>8.91</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
       </c>
       <c r="K7" t="s">
         <v>11</v>
@@ -769,36 +780,48 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>2303</v>
+        <v>2383</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D8">
-        <v>72</v>
+        <v>293.5</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>1.72</v>
       </c>
       <c r="K8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B9">
-        <v>2355</v>
+        <v>2497</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D9">
-        <v>40.450000000000003</v>
+        <v>69.099999999999994</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>4.53</v>
+      </c>
+      <c r="H9">
+        <v>2.95</v>
       </c>
       <c r="K9" t="s">
         <v>11</v>
@@ -806,25 +829,25 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B10">
-        <v>2374</v>
+        <v>3016</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D10">
-        <v>25.45</v>
+        <v>154</v>
       </c>
       <c r="E10">
         <v>3</v>
       </c>
       <c r="F10">
-        <v>8.91</v>
+        <v>5.4</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>4.68</v>
       </c>
       <c r="K10" t="s">
         <v>11</v>
@@ -832,19 +855,25 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B11">
-        <v>2376</v>
+        <v>3037</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D11">
-        <v>148</v>
+        <v>229.5</v>
       </c>
       <c r="E11">
-        <v>2.8</v>
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>2.33</v>
+      </c>
+      <c r="H11">
+        <v>6.22</v>
       </c>
       <c r="K11" t="s">
         <v>11</v>
@@ -852,42 +881,45 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B12">
-        <v>2383</v>
+        <v>3312</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D12">
-        <v>293.5</v>
+        <v>29.05</v>
       </c>
       <c r="E12">
         <v>3</v>
       </c>
-      <c r="F12">
-        <v>1.72</v>
-      </c>
       <c r="K12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B13">
-        <v>2455</v>
+        <v>3532</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="D13">
-        <v>162.5</v>
+        <v>266</v>
       </c>
       <c r="E13">
-        <v>2.5</v>
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>6.71</v>
+      </c>
+      <c r="H13">
+        <v>5.97</v>
       </c>
       <c r="K13" t="s">
         <v>11</v>
@@ -895,42 +927,42 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B14">
-        <v>2476</v>
+        <v>3653</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="D14">
-        <v>69</v>
+        <v>447.5</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>6.07</v>
       </c>
       <c r="K14" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B15">
-        <v>2497</v>
+        <v>4927</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="D15">
-        <v>69.099999999999994</v>
+        <v>114</v>
       </c>
       <c r="E15">
-        <v>3</v>
-      </c>
-      <c r="F15">
-        <v>4.53</v>
-      </c>
-      <c r="H15">
-        <v>2.95</v>
+        <v>2.8</v>
       </c>
       <c r="K15" t="s">
         <v>11</v>
@@ -938,19 +970,25 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="B16">
-        <v>2809</v>
+        <v>6138</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="D16">
-        <v>44.6</v>
+        <v>278.5</v>
       </c>
       <c r="E16">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F16">
+        <v>4.46</v>
+      </c>
+      <c r="H16">
+        <v>3.32</v>
       </c>
       <c r="K16" t="s">
         <v>11</v>
@@ -958,25 +996,25 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="B17">
-        <v>3016</v>
+        <v>6182</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="D17">
-        <v>154</v>
+        <v>88.4</v>
       </c>
       <c r="E17">
         <v>3</v>
       </c>
       <c r="F17">
-        <v>5.4</v>
+        <v>3.65</v>
       </c>
       <c r="H17">
-        <v>4.68</v>
+        <v>12.26</v>
       </c>
       <c r="K17" t="s">
         <v>11</v>
@@ -984,19 +1022,19 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="B18">
-        <v>3017</v>
+        <v>6190</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="D18">
-        <v>92.3</v>
+        <v>39.700000000000003</v>
       </c>
       <c r="E18">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="K18" t="s">
         <v>11</v>
@@ -1004,33 +1042,45 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="B19">
-        <v>3028</v>
+        <v>8069</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="D19">
-        <v>32.700000000000003</v>
+        <v>131</v>
+      </c>
+      <c r="E19">
+        <v>2.9</v>
+      </c>
+      <c r="F19">
+        <v>0.72</v>
+      </c>
+      <c r="H19">
+        <v>6.7</v>
       </c>
       <c r="K19" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B20">
-        <v>3036</v>
+        <v>3169</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D20">
-        <v>69.3</v>
+        <v>283.5</v>
+      </c>
+      <c r="E20">
+        <v>2.9</v>
       </c>
       <c r="K20" t="s">
         <v>8</v>
@@ -1038,42 +1088,39 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="B21">
-        <v>3037</v>
+        <v>6104</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="D21">
-        <v>229.5</v>
+        <v>204.5</v>
       </c>
       <c r="E21">
-        <v>3</v>
-      </c>
-      <c r="F21">
-        <v>2.33</v>
-      </c>
-      <c r="H21">
-        <v>6.22</v>
+        <v>2.9</v>
       </c>
       <c r="K21" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="B22">
-        <v>3122</v>
+        <v>6118</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="D22">
-        <v>72.8</v>
+        <v>31.65</v>
+      </c>
+      <c r="E22">
+        <v>2.9</v>
       </c>
       <c r="K22" t="s">
         <v>8</v>
@@ -1081,36 +1128,39 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="B23">
-        <v>3169</v>
+        <v>6271</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="D23">
-        <v>283.5</v>
+        <v>323.5</v>
+      </c>
+      <c r="E23">
+        <v>2.8</v>
       </c>
       <c r="K23" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="B24">
-        <v>3221</v>
+        <v>8046</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="D24">
-        <v>45.1</v>
+        <v>631</v>
       </c>
       <c r="E24">
-        <v>2.8</v>
+        <v>2.9</v>
       </c>
       <c r="K24" t="s">
         <v>11</v>
@@ -1118,16 +1168,19 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B25">
-        <v>3294</v>
+        <v>3122</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D25">
-        <v>33.25</v>
+        <v>72.8</v>
+      </c>
+      <c r="E25">
+        <v>2.8</v>
       </c>
       <c r="K25" t="s">
         <v>8</v>
@@ -1135,36 +1188,39 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="B26">
-        <v>3306</v>
+        <v>8182</v>
       </c>
       <c r="C26" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="D26">
-        <v>35.9</v>
+        <v>64.5</v>
+      </c>
+      <c r="E26">
+        <v>2.8</v>
       </c>
       <c r="K26" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="B27">
-        <v>3312</v>
+        <v>1722</v>
       </c>
       <c r="C27" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="D27">
-        <v>29.05</v>
+        <v>73.2</v>
       </c>
       <c r="E27">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="K27" t="s">
         <v>11</v>
@@ -1172,16 +1228,16 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B28">
-        <v>3515</v>
+        <v>2376</v>
       </c>
       <c r="C28" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="D28">
-        <v>260.5</v>
+        <v>148</v>
       </c>
       <c r="E28">
         <v>2.8</v>
@@ -1192,25 +1248,19 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B29">
-        <v>3532</v>
+        <v>3017</v>
       </c>
       <c r="C29" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D29">
-        <v>266</v>
+        <v>92.3</v>
       </c>
       <c r="E29">
-        <v>3</v>
-      </c>
-      <c r="F29">
-        <v>6.71</v>
-      </c>
-      <c r="H29">
-        <v>5.97</v>
+        <v>2.8</v>
       </c>
       <c r="K29" t="s">
         <v>11</v>
@@ -1218,16 +1268,16 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B30">
-        <v>3588</v>
+        <v>3221</v>
       </c>
       <c r="C30" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D30">
-        <v>174.5</v>
+        <v>45.1</v>
       </c>
       <c r="E30">
         <v>2.8</v>
@@ -1238,19 +1288,19 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B31">
-        <v>3624</v>
+        <v>3515</v>
       </c>
       <c r="C31" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D31">
-        <v>56.9</v>
+        <v>260.5</v>
       </c>
       <c r="E31">
-        <v>2</v>
+        <v>2.8</v>
       </c>
       <c r="K31" t="s">
         <v>11</v>
@@ -1258,22 +1308,19 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B32">
-        <v>3653</v>
+        <v>3588</v>
       </c>
       <c r="C32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D32">
-        <v>447.5</v>
+        <v>174.5</v>
       </c>
       <c r="E32">
-        <v>3</v>
-      </c>
-      <c r="F32">
-        <v>6.07</v>
+        <v>2.8</v>
       </c>
       <c r="K32" t="s">
         <v>11</v>
@@ -1281,36 +1328,39 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B33">
-        <v>4919</v>
+        <v>6196</v>
       </c>
       <c r="C33" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D33">
-        <v>175</v>
+        <v>165</v>
+      </c>
+      <c r="E33">
+        <v>2.8</v>
       </c>
       <c r="K33" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="B34">
-        <v>4927</v>
+        <v>6411</v>
       </c>
       <c r="C34" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="D34">
-        <v>114</v>
+        <v>302</v>
       </c>
       <c r="E34">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="K34" t="s">
         <v>11</v>
@@ -1318,16 +1368,19 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="B35">
-        <v>4966</v>
+        <v>8289</v>
       </c>
       <c r="C35" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35">
         <v>42</v>
       </c>
-      <c r="D35">
-        <v>2240</v>
+      <c r="E35">
+        <v>3</v>
       </c>
       <c r="K35" t="s">
         <v>11</v>
@@ -1335,56 +1388,59 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="B36">
-        <v>5410</v>
+        <v>2476</v>
       </c>
       <c r="C36" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="D36">
-        <v>28.4</v>
+        <v>69</v>
       </c>
       <c r="E36">
         <v>2.5</v>
       </c>
       <c r="K36" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B37">
-        <v>5483</v>
+        <v>4919</v>
       </c>
       <c r="C37" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D37">
-        <v>225</v>
+        <v>175</v>
       </c>
       <c r="E37">
         <v>2.5</v>
       </c>
       <c r="K37" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B38">
-        <v>5607</v>
+        <v>6235</v>
       </c>
       <c r="C38" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D38">
-        <v>60</v>
+        <v>24.6</v>
+      </c>
+      <c r="E38">
+        <v>2.5</v>
       </c>
       <c r="K38" t="s">
         <v>8</v>
@@ -1392,59 +1448,59 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="B39">
-        <v>6104</v>
+        <v>1709</v>
       </c>
       <c r="C39" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="D39">
-        <v>204.5</v>
+        <v>25.45</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
       </c>
       <c r="K39" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="B40">
-        <v>6118</v>
+        <v>2455</v>
       </c>
       <c r="C40" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="D40">
-        <v>31.65</v>
+        <v>162.5</v>
+      </c>
+      <c r="E40">
+        <v>2.5</v>
       </c>
       <c r="K40" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B41">
-        <v>6138</v>
+        <v>5410</v>
       </c>
       <c r="C41" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D41">
-        <v>278.5</v>
+        <v>28.4</v>
       </c>
       <c r="E41">
-        <v>3</v>
-      </c>
-      <c r="F41">
-        <v>4.46</v>
-      </c>
-      <c r="H41">
-        <v>3.32</v>
+        <v>2.5</v>
       </c>
       <c r="K41" t="s">
         <v>11</v>
@@ -1452,25 +1508,19 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B42">
-        <v>6182</v>
+        <v>5483</v>
       </c>
       <c r="C42" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D42">
-        <v>88.4</v>
+        <v>225</v>
       </c>
       <c r="E42">
-        <v>3</v>
-      </c>
-      <c r="F42">
-        <v>3.65</v>
-      </c>
-      <c r="H42">
-        <v>12.26</v>
+        <v>2</v>
       </c>
       <c r="K42" t="s">
         <v>11</v>
@@ -1478,19 +1528,19 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B43">
-        <v>6190</v>
+        <v>6603</v>
       </c>
       <c r="C43" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D43">
-        <v>39.700000000000003</v>
+        <v>20.7</v>
       </c>
       <c r="E43">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="K43" t="s">
         <v>11</v>
@@ -1498,19 +1548,19 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B44">
-        <v>6191</v>
+        <v>8121</v>
       </c>
       <c r="C44" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="D44">
-        <v>41</v>
+        <v>58.7</v>
       </c>
       <c r="E44">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="K44" t="s">
         <v>11</v>
@@ -1518,19 +1568,19 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B45">
-        <v>6196</v>
+        <v>8183</v>
       </c>
       <c r="C45" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="D45">
-        <v>165</v>
+        <v>69.3</v>
       </c>
       <c r="E45">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="K45" t="s">
         <v>11</v>
@@ -1538,16 +1588,19 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B46">
-        <v>6205</v>
+        <v>6243</v>
       </c>
       <c r="C46" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D46">
-        <v>57.8</v>
+        <v>64.599999999999994</v>
+      </c>
+      <c r="E46">
+        <v>2.4</v>
       </c>
       <c r="K46" t="s">
         <v>11</v>
@@ -1555,16 +1608,19 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B47">
-        <v>6235</v>
+        <v>6275</v>
       </c>
       <c r="C47" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D47">
-        <v>24.6</v>
+        <v>38</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
       </c>
       <c r="K47" t="s">
         <v>8</v>
@@ -1572,39 +1628,39 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B48">
-        <v>6243</v>
+        <v>6533</v>
       </c>
       <c r="C48" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D48">
-        <v>64.599999999999994</v>
+        <v>644</v>
       </c>
       <c r="E48">
-        <v>2.4</v>
+        <v>2</v>
       </c>
       <c r="K48" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="B49">
-        <v>6271</v>
+        <v>2355</v>
       </c>
       <c r="C49" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="D49">
-        <v>323.5</v>
+        <v>40.450000000000003</v>
       </c>
       <c r="E49">
-        <v>2.9</v>
+        <v>2</v>
       </c>
       <c r="K49" t="s">
         <v>11</v>
@@ -1612,36 +1668,39 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="B50">
-        <v>6275</v>
+        <v>2809</v>
       </c>
       <c r="C50" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="D50">
-        <v>38</v>
+        <v>44.6</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
       </c>
       <c r="K50" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="B51">
-        <v>6411</v>
+        <v>3624</v>
       </c>
       <c r="C51" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="D51">
-        <v>302</v>
+        <v>56.9</v>
       </c>
       <c r="E51">
-        <v>2.8</v>
+        <v>2</v>
       </c>
       <c r="K51" t="s">
         <v>11</v>
@@ -1649,36 +1708,39 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B52">
-        <v>6533</v>
+        <v>6191</v>
       </c>
       <c r="C52" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D52">
-        <v>644</v>
+        <v>41</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
       </c>
       <c r="K52" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B53">
-        <v>6603</v>
+        <v>8112</v>
       </c>
       <c r="C53" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D53">
-        <v>20.7</v>
+        <v>49.3</v>
       </c>
       <c r="E53">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="K53" t="s">
         <v>11</v>
@@ -1686,102 +1748,84 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="B54">
-        <v>8046</v>
+        <v>1570</v>
       </c>
       <c r="C54" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="D54">
-        <v>631</v>
-      </c>
-      <c r="E54">
-        <v>2.9</v>
+        <v>25.95</v>
       </c>
       <c r="K54" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="B55">
-        <v>8069</v>
+        <v>1611</v>
       </c>
       <c r="C55" t="s">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="D55">
-        <v>131</v>
-      </c>
-      <c r="E55">
-        <v>3</v>
-      </c>
-      <c r="F55">
-        <v>0.72</v>
-      </c>
-      <c r="H55">
-        <v>6.7</v>
+        <v>16.55</v>
       </c>
       <c r="K55" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="B56">
-        <v>8112</v>
+        <v>2303</v>
       </c>
       <c r="C56" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="D56">
-        <v>49.3</v>
-      </c>
-      <c r="E56">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="K56" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="B57">
-        <v>8121</v>
+        <v>3028</v>
       </c>
       <c r="C57" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="D57">
-        <v>58.7</v>
-      </c>
-      <c r="E57">
-        <v>2.5</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="K57" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="B58">
-        <v>8182</v>
+        <v>3036</v>
       </c>
       <c r="C58" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="D58">
-        <v>64.5</v>
+        <v>69.3</v>
       </c>
       <c r="K58" t="s">
         <v>8</v>
@@ -1789,45 +1833,42 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="B59">
-        <v>8183</v>
+        <v>3294</v>
       </c>
       <c r="C59" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="D59">
-        <v>69.3</v>
-      </c>
-      <c r="E59">
-        <v>2.5</v>
+        <v>33.25</v>
       </c>
       <c r="K59" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="B60">
-        <v>8289</v>
+        <v>4966</v>
       </c>
       <c r="C60" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D60">
-        <v>42</v>
-      </c>
-      <c r="E60">
-        <v>2.8</v>
+        <v>2240</v>
       </c>
       <c r="K60" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:K60">
+    <sortCondition descending="1" ref="E1"/>
+  </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2044,18 +2085,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2078,14 +2119,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A5FA64B-6BE3-4274-B55B-09573D53A114}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C45D471D-425C-48BA-A446-8875887B1B2E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2100,4 +2133,12 @@
     <ds:schemaRef ds:uri="4bb3d3d4-acd0-4d8e-ae87-a4aef309b0b0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A5FA64B-6BE3-4274-B55B-09573D53A114}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>